<commit_message>
Dropdowns for AI prompts
</commit_message>
<xml_diff>
--- a/FWUsefulPageObjects/PageObjects/TestRunner/Dropdowns.xlsx
+++ b/FWUsefulPageObjects/PageObjects/TestRunner/Dropdowns.xlsx
@@ -1,81 +1,102 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Inflectra\InflectraGitProjects\rapise-spira-test\Rapise Academy Git\PageObjects\TestRunner\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD4E605-3288-4DC8-88C2-AD710DA9B5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="2232" windowWidth="18348" windowHeight="14376" xr2:uid="{15EB7710-CF11-4320-819F-7FDB0F0C3D65}"/>
+    <workbookView xWindow="8880" yWindow="2232" windowWidth="18348" windowHeight="14376" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DoAiReport Prompts" sheetId="2" r:id="rId2"/>
+    <sheet name="DoAiReportPy Prompts" sheetId="3" r:id="rId3"/>
+    <sheet name="DoAiReportHtml Prompts" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Draw status for each test case over time. Each test case - is a horizontal sequence of dots.</t>
+  </si>
+  <si>
+    <t>Build a list of failed test cases and their fail reasons.</t>
+  </si>
+  <si>
+    <t>Create a report describing test case failures. Format as table. Group failures of the same test case and reduce the number of lines in the table for same errors.</t>
+  </si>
+  <si>
+    <t>Create a report for this sequence of test runs. Include failures only into a summary table. Also provide analysis for all runs and list unique TestSet names.</t>
+  </si>
+  <si>
+    <t>ExcludeFromAnalysis</t>
+  </si>
+  <si>
+    <t>DoAiReportHtml.query</t>
+  </si>
+  <si>
+    <t>Describe any patterns and regularities you can see in this data.</t>
+  </si>
+  <si>
+    <t>BaseName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discover which test cases have at least one non-pass status (build an array). Go again through all data and capture available runs of these test cases. Draw all statuses (including Pass, etc.) for each such test case over time. Each test case - is a horizontal sequence of dots. </t>
+  </si>
+  <si>
+    <t>Discover which test cases have at least one non-pass status (build an array). Go again through all data and capture available runs of these test cases. Draw all statuses (including Pass, etc.) for each such test case over time. Each test case - is a horizontal sequence of dots.</t>
+  </si>
+  <si>
+    <t>DoAiReportPy.query</t>
+  </si>
+  <si>
+    <t>Build a table describing failed test cases.</t>
+  </si>
+  <si>
+    <t>What are the top 10 longest test runs?</t>
+  </si>
+  <si>
+    <t>DoAiReport.query</t>
+  </si>
+  <si>
+    <t>Find groups of test cases that usually fail together.</t>
+  </si>
+  <si>
+    <t>MinNumberOfTestRuns</t>
+  </si>
+  <si>
+    <t>Draw fail status for each test case over time. Each test case - is a horizontal sequence of dots. Do not draw Pass points.</t>
+  </si>
   <si>
     <t>TestRunner.SetParameter.name</t>
   </si>
   <si>
-    <t>ExcludeFromAnalysis</t>
-  </si>
-  <si>
-    <t>MinNumberOfTestRuns</t>
-  </si>
-  <si>
-    <t>BaseName</t>
+    <t>Do you observe any anomalies in this test run data?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
+      <name val="Aptos Narrow"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
       <b/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
+      <color rgb="FF333333"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,7 +108,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border outline="0">
       <left/>
       <right/>
       <top/>
@@ -98,24 +119,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -435,39 +449,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EED480C-765C-4DFE-BF76-DFB63C662B5A}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$A$4" sqref="$A$4:$XFD$4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$A$2" sqref="$A$2:$A$9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="151.796875" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$A$2" sqref="$A$2:$A$4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="145.49609375" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$A$2" sqref="$A$2:$A$2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="115.296875" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>